<commit_message>
tickets #10 #11 #3
</commit_message>
<xml_diff>
--- a/documentos/atualizacao-13-01.xlsx
+++ b/documentos/atualizacao-13-01.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504ABEF5-B844-4EDE-890B-40FE976E04B3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903C0C6D-3BF3-491D-B0EC-739C7440FB50}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Em "Entidades", a opção "Cor" deve vir em primeiro, já que ela trava as outras. </t>
   </si>
@@ -40,22 +40,19 @@
     <t>Observação</t>
   </si>
   <si>
-    <t>Não consegui reproduzir</t>
-  </si>
-  <si>
     <t>Aba de estoque</t>
   </si>
   <si>
     <t>Na tela de Criar Produto, o item preço não se aplica e a "quantidade estoque" deve ser preenchida automaticamente, de acordo coma quantidade inicial cadastrada (sendo ajustada com as entrada e saídas)</t>
   </si>
   <si>
-    <t>É necessário informar o preço do Produto. Caso contrário não será possível calcular o preço de um Pedido.</t>
-  </si>
-  <si>
     <t>Em Material, ao pesquisar um material nada acontece.</t>
   </si>
   <si>
-    <t>Por quê é necessário ter uma aba de estoque? Sendo que já existe um campo de estoque no Produto</t>
+    <t>Já estava implementado o que seria necessário para o cliente. Talvez ele peça uma no funcionadade</t>
+  </si>
+  <si>
+    <t>É necessário informar o preço do Produto. O usuário está confundindo o dinheiro do adiantamento na tela de Pedido, com o valor do proço do Produto.</t>
   </si>
 </sst>
 </file>
@@ -78,7 +75,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,19 +90,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -122,22 +107,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -420,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
@@ -441,48 +420,48 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>9</v>
-      </c>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>